<commit_message>
Add members to SC
Added Dr. Mohri, Ishida, Nonaka to the scientific committee.
</commit_message>
<xml_diff>
--- a/content/people/SCmemberList.xlsx
+++ b/content/people/SCmemberList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/tristan2025-website/content/people/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAFAEEB-DA5F-6446-8477-B775F89F9E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348CB162-993C-4244-A9C8-727D92D1AD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="340">
   <si>
     <t>Name</t>
   </si>
@@ -1075,6 +1075,26 @@
   </si>
   <si>
     <t>Université Sorbonne Paris Nord</t>
+  </si>
+  <si>
+    <t>Yuichi Mohri</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>The Institute of Behavioral Sciences</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Takashi Ishida</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Highway Planning Inc.</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Yasuhiro Nonaka</t>
+    <phoneticPr fontId="11"/>
   </si>
 </sst>
 </file>
@@ -1558,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A162" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -3825,6 +3845,39 @@
       </c>
       <c r="C174" s="12" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>335</v>
+      </c>
+      <c r="B175" t="s">
+        <v>336</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>337</v>
+      </c>
+      <c r="B176" t="s">
+        <v>338</v>
+      </c>
+      <c r="C176" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>339</v>
+      </c>
+      <c r="B177" t="s">
+        <v>338</v>
+      </c>
+      <c r="C177" s="11" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Latifa Oukhellou to SC
</commit_message>
<xml_diff>
--- a/content/people/SCmemberList.xlsx
+++ b/content/people/SCmemberList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348CB162-993C-4244-A9C8-727D92D1AD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3F582D-EC2E-394A-B5D5-5851BF3D1A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="342">
   <si>
     <t>Name</t>
   </si>
@@ -1094,6 +1094,14 @@
   </si>
   <si>
     <t>Yasuhiro Nonaka</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Université Gustave Eiffel</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Latifa Oukhellou</t>
     <phoneticPr fontId="11"/>
   </si>
 </sst>
@@ -1578,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A162" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -3878,6 +3886,17 @@
       </c>
       <c r="C177" s="11" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>341</v>
+      </c>
+      <c r="B178" t="s">
+        <v>340</v>
+      </c>
+      <c r="C178" s="11" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add two members to SC
</commit_message>
<xml_diff>
--- a/content/people/SCmemberList.xlsx
+++ b/content/people/SCmemberList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5934CDD0-F34C-8B40-9BEC-C6680316D030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60C25B4-77EA-774B-A75F-F5DFDDFFC86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="341">
   <si>
     <t>Name</t>
   </si>
@@ -1091,6 +1091,14 @@
   </si>
   <si>
     <t>Rotterdam School of Managament, Erasmus University</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Mutsunori Yagiura</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Nur Diana Safitri</t>
     <phoneticPr fontId="11"/>
   </si>
 </sst>
@@ -1575,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177:XFD177"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -3861,6 +3869,28 @@
         <v>336</v>
       </c>
       <c r="C176" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>339</v>
+      </c>
+      <c r="B177" t="s">
+        <v>213</v>
+      </c>
+      <c r="C177" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>340</v>
+      </c>
+      <c r="B178" t="s">
+        <v>202</v>
+      </c>
+      <c r="C178" s="11" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add cortes to sc
</commit_message>
<xml_diff>
--- a/content/people/SCmemberList.xlsx
+++ b/content/people/SCmemberList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EAB725-1BC0-1243-8B6C-83617F6C8528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C226FC5-62CC-5141-AF6F-0FFEFC8061FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="347">
   <si>
     <t>Name</t>
   </si>
@@ -1110,6 +1110,18 @@
   </si>
   <si>
     <t>Portugal</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Cristián E. Cortés</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Universidad de Chile</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Chile</t>
     <phoneticPr fontId="11"/>
   </si>
 </sst>
@@ -1594,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A165" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -3914,6 +3926,17 @@
       </c>
       <c r="C179" s="11" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>344</v>
+      </c>
+      <c r="B180" t="s">
+        <v>345</v>
+      </c>
+      <c r="C180" s="11" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>